<commit_message>
Mapa de 14 niveles
</commit_message>
<xml_diff>
--- a/01_Documentos/Grupo3_Mapa de procesos 14 niveles.xlsx
+++ b/01_Documentos/Grupo3_Mapa de procesos 14 niveles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivobook Oled\Desktop\Universidad\Septimo Semestre\Aseguramiento\Unidad 1\2563_G3_ACSW\01_Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DA9E16-66E1-425E-9ADF-6FECF6963258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DE6E7F-FA9F-4694-AFD2-D337BCC956C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05AC8D40-0673-44FF-B842-F2CFFFBC4894}"/>
   </bookViews>
@@ -3248,8 +3248,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5778211" y="8202138"/>
-          <a:ext cx="1323975" cy="1065687"/>
+          <a:off x="5798004" y="8316142"/>
+          <a:ext cx="1323975" cy="1082312"/>
           <a:chOff x="9484702" y="2765066"/>
           <a:chExt cx="1089646" cy="1074767"/>
         </a:xfrm>
@@ -3561,8 +3561,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9674753" y="8192616"/>
-          <a:ext cx="1343940" cy="1094259"/>
+          <a:off x="9723838" y="8306620"/>
+          <a:ext cx="1343940" cy="1110884"/>
           <a:chOff x="9535756" y="2889558"/>
           <a:chExt cx="589065" cy="1246449"/>
         </a:xfrm>
@@ -4475,8 +4475,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7703127" y="8187170"/>
-          <a:ext cx="1371600" cy="1080655"/>
+          <a:off x="7737566" y="8301174"/>
+          <a:ext cx="1371600" cy="1097280"/>
           <a:chOff x="9535756" y="2889558"/>
           <a:chExt cx="589065" cy="1246449"/>
         </a:xfrm>
@@ -4813,8 +4813,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3824304" y="8124221"/>
-          <a:ext cx="1385005" cy="520866"/>
+          <a:off x="3829450" y="8238225"/>
+          <a:ext cx="1391339" cy="529178"/>
           <a:chOff x="9535756" y="2889556"/>
           <a:chExt cx="589065" cy="926671"/>
         </a:xfrm>
@@ -5151,8 +5151,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3828033" y="8729218"/>
-          <a:ext cx="1323975" cy="534256"/>
+          <a:off x="3833179" y="8851534"/>
+          <a:ext cx="1323975" cy="542569"/>
           <a:chOff x="9525602" y="2701934"/>
           <a:chExt cx="1089646" cy="538729"/>
         </a:xfrm>
@@ -5452,8 +5452,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7128479" y="5602053"/>
-          <a:ext cx="546939" cy="2331893"/>
+          <a:off x="7148272" y="5677264"/>
+          <a:ext cx="558814" cy="2367915"/>
           <a:chOff x="10126135" y="5820833"/>
           <a:chExt cx="533399" cy="2741084"/>
         </a:xfrm>
@@ -5629,8 +5629,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11016899" y="5624196"/>
-          <a:ext cx="546939" cy="2331893"/>
+          <a:off x="11065984" y="5699407"/>
+          <a:ext cx="558814" cy="2367915"/>
           <a:chOff x="10126135" y="5820833"/>
           <a:chExt cx="533399" cy="2741084"/>
         </a:xfrm>
@@ -5933,8 +5933,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11682337" y="8747148"/>
-          <a:ext cx="1358816" cy="534256"/>
+          <a:off x="11746068" y="8869464"/>
+          <a:ext cx="1365149" cy="542569"/>
           <a:chOff x="9525602" y="2701934"/>
           <a:chExt cx="1089646" cy="538729"/>
         </a:xfrm>
@@ -6352,19 +6352,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>M</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-EC" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>ide si se mantiene el nivel mínimo requerido de existencias (2 pacas por producto) para asegurar la disponibilidad continua de productos.</a:t>
+            <a:t>Mantener al menos 2 pacas de cada producto en inventario.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7498,7 +7486,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="MP14niveles!$C$9:$AY$85" spid="_x0000_s2083"/>
+                  <a14:cameraTool cellRange="MP14niveles!$C$9:$AY$85" spid="_x0000_s2084"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7840,7 +7828,7 @@
   </sheetPr>
   <dimension ref="C12:AY86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P80" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="55" workbookViewId="0">
       <selection activeCell="DX108" sqref="DX108"/>
     </sheetView>
   </sheetViews>
@@ -7965,14 +7953,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B370B9D439DDE546813D90F3B8B4DBAB" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="512b45069a73f00acf967ec99d7533f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xmlns:ns4="a8c64c2c-2712-4198-95b2-d256c44e1621" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5eb5ad93516d041cc0acfadbac38bba" ns3:_="" ns4:_="">
     <xsd:import namespace="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
@@ -8219,6 +8199,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8229,16 +8217,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E070C3-B3EF-4CFE-A975-5E4131163DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E52A94-29CD-49E2-93D5-AA07EA39528B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8257,6 +8235,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E070C3-B3EF-4CFE-A975-5E4131163DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8F17B7-1194-404B-B4BE-AE81FE298C94}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Modificacion del mapa de 14 niveles
</commit_message>
<xml_diff>
--- a/01_Documentos/Grupo3_Mapa de procesos 14 niveles.xlsx
+++ b/01_Documentos/Grupo3_Mapa de procesos 14 niveles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivobook Oled\Desktop\Universidad\Septimo Semestre\Aseguramiento\Unidad 1\2563_G3_ACSW\01_Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DE6E7F-FA9F-4694-AFD2-D337BCC956C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B7569B-0627-4F76-B6AB-EE45C1043150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05AC8D40-0673-44FF-B842-F2CFFFBC4894}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>UNIVERSIDAD DE LAS FUERZAS ARMADAS UFA - ESPE
-MAPA DE PROCESOS DE 10 NIVELES PARA EL MODELO DE NEGOCIO ACTUAL DEL CONTROL DE INVENTARIO DE BAZAR Y PAPELERÍA</t>
+MAPA DE PROCESOS DE 14 NIVELES PARA EL MODELO DE NEGOCIO ACTUAL DEL CONTROL DE INVENTARIO DE BAZAR Y PAPELERÍA</t>
   </si>
 </sst>
 </file>
@@ -125,22 +125,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>67997</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>117049</xdr:rowOff>
+      <xdr:colOff>59599</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>46089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>69273</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:colOff>51954</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>46090</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectángulo: esquinas redondeadas 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF3D9091-E709-4A15-A76E-66701866ECB1}"/>
+        <xdr:cNvPr id="144" name="Rectángulo: esquinas redondeadas 143">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE956154-A610-4786-9862-AADFE91121B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -148,8 +148,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1003179" y="5364458"/>
-          <a:ext cx="13821185" cy="4468558"/>
+          <a:off x="994781" y="3007498"/>
+          <a:ext cx="13812264" cy="952501"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -189,18 +189,8 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="es-EC" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>+</a:t>
-          </a:r>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-EC" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -209,22 +199,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>59599</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>46089</xdr:rowOff>
+      <xdr:colOff>66599</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>122463</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>51954</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>46090</xdr:rowOff>
+      <xdr:colOff>121227</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>68034</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="144" name="Rectángulo: esquinas redondeadas 143">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE956154-A610-4786-9862-AADFE91121B3}"/>
+        <xdr:cNvPr id="145" name="Rectángulo: esquinas redondeadas 144">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{590F84FE-7AFD-4217-A0EA-87AB8BCE3429}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -232,8 +222,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="994781" y="3007498"/>
-          <a:ext cx="13812264" cy="952501"/>
+          <a:off x="1005492" y="10695213"/>
+          <a:ext cx="13961128" cy="1469571"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -273,80 +263,6 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-EC" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>66599</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>122463</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>121227</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>68034</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="145" name="Rectángulo: esquinas redondeadas 144">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{590F84FE-7AFD-4217-A0EA-87AB8BCE3429}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1005492" y="10695213"/>
-          <a:ext cx="13961128" cy="1469571"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="85000"/>
-            <a:alpha val="20000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="85000"/>
-              <a:alpha val="98000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
           <a:endParaRPr lang="es-EC" sz="1100">
             <a:solidFill>
@@ -2731,7 +2647,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="es-EC" baseline="0"/>
-            <a:t> (Entradas y salidad</a:t>
+            <a:t> (Entradas y salidas</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-EC"/>
@@ -3224,16 +3140,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>64295</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>138793</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:rowOff>162606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>7145</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>147638</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3248,8 +3164,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5798004" y="8316142"/>
-          <a:ext cx="1323975" cy="1082312"/>
+          <a:off x="9753418" y="8292560"/>
+          <a:ext cx="1361342" cy="1075278"/>
           <a:chOff x="9484702" y="2765066"/>
           <a:chExt cx="1089646" cy="1074767"/>
         </a:xfrm>
@@ -3293,20 +3209,8 @@
           <a:lstStyle/>
           <a:p>
             <a:r>
-              <a:rPr lang="es-EC" sz="1100" b="0" i="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1"/>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>Instructivo </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="es-EC"/>
-              <a:t>para cálculo de necesidades de reabastecimiento</a:t>
+              <a:t>Resolución NAC-DGERCGC12-00105 del SRI</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -3537,357 +3441,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>18135</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>129271</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="155" name="Grupo 154">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C0C1E93-D030-45F4-B613-A6721F1AA9B8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="9723838" y="8306620"/>
-          <a:ext cx="1343940" cy="1110884"/>
-          <a:chOff x="9535756" y="2889558"/>
-          <a:chExt cx="589065" cy="1246449"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="156" name="Rectángulo 155">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CDAF505-3B52-4417-A957-C161EE0F9B88}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9535756" y="2889558"/>
-            <a:ext cx="589065" cy="999135"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5">
-              <a:tint val="50000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5">
-              <a:tint val="50000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="es-EC">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Procedimiento de recepción de</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-EC" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> pedidos</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-EC">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="157" name="Forma libre: forma 156">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA8C26AF-17E1-46A2-BB6A-4C1A498A0736}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9538404" y="3828211"/>
-            <a:ext cx="498854" cy="307796"/>
-          </a:xfrm>
-          <a:custGeom>
-            <a:avLst/>
-            <a:gdLst>
-              <a:gd name="connsiteX0" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY0" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX1" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY1" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX2" fmla="*/ 652073 w 928218"/>
-              <a:gd name="connsiteY2" fmla="*/ -31246 h 292023"/>
-              <a:gd name="connsiteX3" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY3" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX4" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY4" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX5" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY5" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX6" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY6" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX7" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY7" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX8" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY8" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX9" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY9" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX10" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY10" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX11" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY11" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX12" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY12" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX13" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY13" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX14" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY14" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX15" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY15" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX16" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY16" fmla="*/ 0 h 292023"/>
-            </a:gdLst>
-            <a:ahLst/>
-            <a:cxnLst>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX0" y="connsiteY0"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX1" y="connsiteY1"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX2" y="connsiteY2"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX3" y="connsiteY3"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX4" y="connsiteY4"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX5" y="connsiteY5"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX6" y="connsiteY6"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX7" y="connsiteY7"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX8" y="connsiteY8"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX9" y="connsiteY9"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX10" y="connsiteY10"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX11" y="connsiteY11"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX12" y="connsiteY12"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX13" y="connsiteY13"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX14" y="connsiteY14"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX15" y="connsiteY15"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX16" y="connsiteY16"/>
-              </a:cxn>
-            </a:cxnLst>
-            <a:rect l="l" t="t" r="r" b="b"/>
-            <a:pathLst>
-              <a:path w="928218" h="292023">
-                <a:moveTo>
-                  <a:pt x="0" y="0"/>
-                </a:moveTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="652073" y="-31246"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="0"/>
-                </a:lnTo>
-                <a:close/>
-              </a:path>
-            </a:pathLst>
-          </a:custGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
-              <a:lnSpc>
-                <a:spcPct val="90000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPct val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPct val="35000"/>
-              </a:spcAft>
-              <a:buNone/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-EC" sz="1300" kern="1200"/>
-              <a:t>PD</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
@@ -4086,7 +3639,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="es-EC" sz="1100"/>
-            <a:t>8 Dìa</a:t>
+            <a:t>1 Día</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4451,23 +4004,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1378843</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>60235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>50710</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="183" name="Grupo 182">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C552746-9F6B-4657-89A6-83A9CDC167B3}"/>
+        <xdr:cNvPr id="20" name="Grupo 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C69621A2-21C4-4F12-AE13-72E70C50507E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4475,985 +4028,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7737566" y="8301174"/>
-          <a:ext cx="1371600" cy="1097280"/>
-          <a:chOff x="9535756" y="2889558"/>
-          <a:chExt cx="589065" cy="1246449"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="184" name="Rectángulo 183">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92CF7649-A024-498F-AB35-7E66CFF2F53C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9535756" y="2889558"/>
-            <a:ext cx="589065" cy="999135"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5">
-              <a:tint val="50000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5">
-              <a:tint val="50000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="es-EC">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Procedimiento de generación de pedidos</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="185" name="Forma libre: forma 184">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7048C20A-D6E0-4948-B057-F5A2523780AD}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9538407" y="3833053"/>
-            <a:ext cx="498854" cy="302954"/>
-          </a:xfrm>
-          <a:custGeom>
-            <a:avLst/>
-            <a:gdLst>
-              <a:gd name="connsiteX0" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY0" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX1" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY1" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX2" fmla="*/ 652073 w 928218"/>
-              <a:gd name="connsiteY2" fmla="*/ -31246 h 292023"/>
-              <a:gd name="connsiteX3" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY3" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX4" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY4" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX5" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY5" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX6" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY6" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX7" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY7" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX8" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY8" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX9" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY9" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX10" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY10" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX11" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY11" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX12" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY12" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX13" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY13" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX14" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY14" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX15" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY15" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX16" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY16" fmla="*/ 0 h 292023"/>
-            </a:gdLst>
-            <a:ahLst/>
-            <a:cxnLst>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX0" y="connsiteY0"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX1" y="connsiteY1"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX2" y="connsiteY2"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX3" y="connsiteY3"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX4" y="connsiteY4"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX5" y="connsiteY5"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX6" y="connsiteY6"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX7" y="connsiteY7"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX8" y="connsiteY8"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX9" y="connsiteY9"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX10" y="connsiteY10"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX11" y="connsiteY11"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX12" y="connsiteY12"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX13" y="connsiteY13"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX14" y="connsiteY14"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX15" y="connsiteY15"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX16" y="connsiteY16"/>
-              </a:cxn>
-            </a:cxnLst>
-            <a:rect l="l" t="t" r="r" b="b"/>
-            <a:pathLst>
-              <a:path w="928218" h="292023">
-                <a:moveTo>
-                  <a:pt x="0" y="0"/>
-                </a:moveTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="652073" y="-31246"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="0"/>
-                </a:lnTo>
-                <a:close/>
-              </a:path>
-            </a:pathLst>
-          </a:custGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
-              <a:lnSpc>
-                <a:spcPct val="90000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPct val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPct val="35000"/>
-              </a:spcAft>
-              <a:buNone/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-EC" sz="1300" kern="1200"/>
-              <a:t>PD</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28159</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>60876</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>41414</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="12" name="Grupo 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38B59C25-0F6D-4A41-BDE6-5DE344439B94}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="3829450" y="8238225"/>
-          <a:ext cx="1391339" cy="529178"/>
-          <a:chOff x="9535756" y="2889556"/>
-          <a:chExt cx="589065" cy="926671"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="Rectángulo 12">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1660443-BEEF-AA28-59DF-1AA693AAD0BE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9535756" y="2889556"/>
-            <a:ext cx="589065" cy="664740"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5">
-              <a:tint val="50000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5">
-              <a:tint val="50000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="es-EC" sz="900">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Procedimiento de revisión de inventario</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="Forma libre: forma 13">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B17B91BB-9ACF-CAB2-76B2-5C9B94ECDB5A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9538407" y="3513273"/>
-            <a:ext cx="498854" cy="302954"/>
-          </a:xfrm>
-          <a:custGeom>
-            <a:avLst/>
-            <a:gdLst>
-              <a:gd name="connsiteX0" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY0" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX1" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY1" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX2" fmla="*/ 652073 w 928218"/>
-              <a:gd name="connsiteY2" fmla="*/ -31246 h 292023"/>
-              <a:gd name="connsiteX3" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY3" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX4" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY4" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX5" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY5" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX6" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY6" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX7" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY7" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX8" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY8" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX9" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY9" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX10" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY10" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX11" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY11" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX12" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY12" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX13" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY13" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX14" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY14" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX15" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY15" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX16" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY16" fmla="*/ 0 h 292023"/>
-            </a:gdLst>
-            <a:ahLst/>
-            <a:cxnLst>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX0" y="connsiteY0"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX1" y="connsiteY1"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX2" y="connsiteY2"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX3" y="connsiteY3"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX4" y="connsiteY4"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX5" y="connsiteY5"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX6" y="connsiteY6"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX7" y="connsiteY7"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX8" y="connsiteY8"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX9" y="connsiteY9"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX10" y="connsiteY10"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX11" y="connsiteY11"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX12" y="connsiteY12"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX13" y="connsiteY13"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX14" y="connsiteY14"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX15" y="connsiteY15"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX16" y="connsiteY16"/>
-              </a:cxn>
-            </a:cxnLst>
-            <a:rect l="l" t="t" r="r" b="b"/>
-            <a:pathLst>
-              <a:path w="928218" h="292023">
-                <a:moveTo>
-                  <a:pt x="0" y="0"/>
-                </a:moveTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="652073" y="-31246"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="0"/>
-                </a:lnTo>
-                <a:close/>
-              </a:path>
-            </a:pathLst>
-          </a:custGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
-              <a:lnSpc>
-                <a:spcPct val="90000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPct val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPct val="35000"/>
-              </a:spcAft>
-              <a:buNone/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-EC" sz="1300" kern="1200"/>
-              <a:t>PD</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>31888</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>125545</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1355863</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>119474</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="15" name="Grupo 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC2EE5F5-5F1E-4705-94DF-E6FAF2E4011E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="3833179" y="8851534"/>
-          <a:ext cx="1323975" cy="542569"/>
-          <a:chOff x="9525602" y="2701934"/>
-          <a:chExt cx="1089646" cy="538729"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="16" name="Rectángulo 15">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DCC06F1-CC23-2D38-5F69-0A4FEFF7E5C4}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9525602" y="2701934"/>
-            <a:ext cx="1089646" cy="377301"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:lnRef>
-          <a:fillRef idx="2">
-            <a:schemeClr val="accent5"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="es-EC" sz="900"/>
-              <a:t>Instructivo para registro en libreta de inventario</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="19" name="Forma libre: forma 18">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D80D79E-7A01-560E-C5F7-79C26C0C5F70}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9592198" y="3034863"/>
-            <a:ext cx="928218" cy="205800"/>
-          </a:xfrm>
-          <a:custGeom>
-            <a:avLst/>
-            <a:gdLst>
-              <a:gd name="connsiteX0" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY0" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX1" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY1" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX2" fmla="*/ 652073 w 928218"/>
-              <a:gd name="connsiteY2" fmla="*/ -31246 h 292023"/>
-              <a:gd name="connsiteX3" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY3" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX4" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY4" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX5" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY5" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX6" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY6" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX7" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY7" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX8" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY8" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX9" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY9" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX10" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY10" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX11" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY11" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX12" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY12" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX13" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY13" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX14" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY14" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX15" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY15" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX16" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY16" fmla="*/ 0 h 292023"/>
-            </a:gdLst>
-            <a:ahLst/>
-            <a:cxnLst>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX0" y="connsiteY0"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX1" y="connsiteY1"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX2" y="connsiteY2"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX3" y="connsiteY3"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX4" y="connsiteY4"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX5" y="connsiteY5"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX6" y="connsiteY6"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX7" y="connsiteY7"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX8" y="connsiteY8"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX9" y="connsiteY9"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX10" y="connsiteY10"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX11" y="connsiteY11"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX12" y="connsiteY12"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX13" y="connsiteY13"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX14" y="connsiteY14"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX15" y="connsiteY15"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX16" y="connsiteY16"/>
-              </a:cxn>
-            </a:cxnLst>
-            <a:rect l="l" t="t" r="r" b="b"/>
-            <a:pathLst>
-              <a:path w="928218" h="292023">
-                <a:moveTo>
-                  <a:pt x="0" y="0"/>
-                </a:moveTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="652073" y="-31246"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="0"/>
-                </a:lnTo>
-                <a:close/>
-              </a:path>
-            </a:pathLst>
-          </a:custGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
-              <a:lnSpc>
-                <a:spcPct val="90000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPct val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPct val="35000"/>
-              </a:spcAft>
-              <a:buNone/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-EC" sz="1300" kern="1200"/>
-              <a:t>IT</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1378843</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>60235</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>50710</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="20" name="Grupo 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C69621A2-21C4-4F12-AE13-72E70C50507E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="7148272" y="5677264"/>
-          <a:ext cx="558814" cy="2367915"/>
+          <a:off x="7140735" y="5646281"/>
+          <a:ext cx="555465" cy="2352675"/>
           <a:chOff x="10126135" y="5820833"/>
           <a:chExt cx="533399" cy="2741084"/>
         </a:xfrm>
@@ -5629,8 +4205,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11065984" y="5699407"/>
-          <a:ext cx="558814" cy="2367915"/>
+          <a:off x="11049404" y="5668424"/>
+          <a:ext cx="555465" cy="2352675"/>
           <a:chOff x="10126135" y="5820833"/>
           <a:chExt cx="533399" cy="2741084"/>
         </a:xfrm>
@@ -5909,307 +4485,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>72228</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>143475</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>17880</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>137404</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="36" name="Grupo 35">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E44F25C9-231B-4259-89B8-EDD932D8644D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="11746068" y="8869464"/>
-          <a:ext cx="1365149" cy="542569"/>
-          <a:chOff x="9525602" y="2701934"/>
-          <a:chExt cx="1089646" cy="538729"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="37" name="Rectángulo 36">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36E65726-48CC-1E5D-3D41-3A6E855C29F8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9525602" y="2701934"/>
-            <a:ext cx="1089646" cy="377301"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:lnRef>
-          <a:fillRef idx="2">
-            <a:schemeClr val="accent5"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="es-EC" sz="900"/>
-              <a:t>Instructivo para registro en libreta de inventario</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="50" name="Forma libre: forma 49">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ED6CFD7-3D7F-7B8C-7688-58B20A20A4B2}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9592198" y="3034863"/>
-            <a:ext cx="928218" cy="205800"/>
-          </a:xfrm>
-          <a:custGeom>
-            <a:avLst/>
-            <a:gdLst>
-              <a:gd name="connsiteX0" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY0" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX1" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY1" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX2" fmla="*/ 652073 w 928218"/>
-              <a:gd name="connsiteY2" fmla="*/ -31246 h 292023"/>
-              <a:gd name="connsiteX3" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY3" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX4" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY4" fmla="*/ 0 h 292023"/>
-              <a:gd name="connsiteX5" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY5" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX6" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY6" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX7" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY7" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX8" fmla="*/ 928218 w 928218"/>
-              <a:gd name="connsiteY8" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX9" fmla="*/ 773515 w 928218"/>
-              <a:gd name="connsiteY9" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX10" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY10" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX11" fmla="*/ 541461 w 928218"/>
-              <a:gd name="connsiteY11" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX12" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY12" fmla="*/ 292023 h 292023"/>
-              <a:gd name="connsiteX13" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY13" fmla="*/ 121676 h 292023"/>
-              <a:gd name="connsiteX14" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY14" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX15" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY15" fmla="*/ 48671 h 292023"/>
-              <a:gd name="connsiteX16" fmla="*/ 0 w 928218"/>
-              <a:gd name="connsiteY16" fmla="*/ 0 h 292023"/>
-            </a:gdLst>
-            <a:ahLst/>
-            <a:cxnLst>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX0" y="connsiteY0"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX1" y="connsiteY1"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX2" y="connsiteY2"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX3" y="connsiteY3"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX4" y="connsiteY4"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX5" y="connsiteY5"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX6" y="connsiteY6"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX7" y="connsiteY7"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX8" y="connsiteY8"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX9" y="connsiteY9"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX10" y="connsiteY10"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX11" y="connsiteY11"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX12" y="connsiteY12"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX13" y="connsiteY13"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX14" y="connsiteY14"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX15" y="connsiteY15"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="connsiteX16" y="connsiteY16"/>
-              </a:cxn>
-            </a:cxnLst>
-            <a:rect l="l" t="t" r="r" b="b"/>
-            <a:pathLst>
-              <a:path w="928218" h="292023">
-                <a:moveTo>
-                  <a:pt x="0" y="0"/>
-                </a:moveTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="652073" y="-31246"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="928218" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="773515" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="541461" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="292023"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="121676"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="48671"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="0"/>
-                </a:lnTo>
-                <a:close/>
-              </a:path>
-            </a:pathLst>
-          </a:custGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
-              <a:lnSpc>
-                <a:spcPct val="90000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPct val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPct val="35000"/>
-              </a:spcAft>
-              <a:buNone/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-EC" sz="1300" kern="1200"/>
-              <a:t>IT</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>4484</xdr:colOff>
       <xdr:row>77</xdr:row>
@@ -6330,6 +4605,7 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr rtl="0"/>
           <a:r>
             <a:rPr lang="es-EC" sz="1100" b="1" i="0" baseline="0">
               <a:solidFill>
@@ -6343,7 +4619,7 @@
             <a:t>Meta: </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-EC" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="es-EC" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6354,6 +4630,9 @@
             </a:rPr>
             <a:t>Mantener al menos 2 pacas de cada producto en inventario.</a:t>
           </a:r>
+          <a:endParaRPr lang="es-EC" b="0">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -6933,7 +5212,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="es-EC" sz="1100" b="1"/>
-            <a:t>Nivel  10. Inidicadores</a:t>
+            <a:t>Nivel  10. Indicadores</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7394,16 +5673,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>22861</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>73163</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>115965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>537882</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>75162</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>527685</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7433,8 +5712,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9540241" y="16945842"/>
-          <a:ext cx="2653664" cy="324888"/>
+          <a:off x="9161134" y="17272171"/>
+          <a:ext cx="2739513" cy="365888"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7486,7 +5765,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="MP14niveles!$C$9:$AY$85" spid="_x0000_s2084"/>
+                  <a14:cameraTool cellRange="MP14niveles!$C$9:$AY$85" spid="_x0000_s2091"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7828,8 +6107,8 @@
   </sheetPr>
   <dimension ref="C12:AY86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P80" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="DX108" sqref="DX108"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="AF66" sqref="AF66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7953,6 +6232,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B370B9D439DDE546813D90F3B8B4DBAB" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="512b45069a73f00acf967ec99d7533f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xmlns:ns4="a8c64c2c-2712-4198-95b2-d256c44e1621" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5eb5ad93516d041cc0acfadbac38bba" ns3:_="" ns4:_="">
     <xsd:import namespace="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
@@ -8199,14 +6486,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8217,6 +6496,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E070C3-B3EF-4CFE-A975-5E4131163DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E52A94-29CD-49E2-93D5-AA07EA39528B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8235,16 +6524,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E070C3-B3EF-4CFE-A975-5E4131163DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8F17B7-1194-404B-B4BE-AE81FE298C94}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
modificacion en el mapa
</commit_message>
<xml_diff>
--- a/01_Documentos/Grupo3_Mapa de procesos 14 niveles.xlsx
+++ b/01_Documentos/Grupo3_Mapa de procesos 14 niveles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivobook Oled\Desktop\Universidad\Septimo Semestre\Aseguramiento\Unidad 1\2563_G3_ACSW\01_Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6015F30F-B164-4DCC-8C2E-C7ADED3E62D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B23B26-CEFB-4441-9081-CC991F2CEB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05AC8D40-0673-44FF-B842-F2CFFFBC4894}"/>
   </bookViews>
@@ -3164,8 +3164,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9781109" y="8381696"/>
-          <a:ext cx="1361746" cy="1088618"/>
+          <a:off x="9782453" y="8395750"/>
+          <a:ext cx="1360525" cy="1090818"/>
           <a:chOff x="9484702" y="2765066"/>
           <a:chExt cx="1089646" cy="1074767"/>
         </a:xfrm>
@@ -4028,8 +4028,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7154277" y="5704290"/>
-          <a:ext cx="560316" cy="2381579"/>
+          <a:off x="7155866" y="5713212"/>
+          <a:ext cx="559827" cy="2386345"/>
           <a:chOff x="10126135" y="5820833"/>
           <a:chExt cx="533399" cy="2741084"/>
         </a:xfrm>
@@ -4205,8 +4205,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11077095" y="5726433"/>
-          <a:ext cx="560315" cy="2381579"/>
+          <a:off x="11078439" y="5735355"/>
+          <a:ext cx="559827" cy="2386345"/>
           <a:chOff x="10126135" y="5820833"/>
           <a:chExt cx="533399" cy="2741084"/>
         </a:xfrm>
@@ -4575,8 +4575,29 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Nivel de Existencias Adecuado</a:t>
-          </a:r>
+            <a:t>Nivel de Existencias Adecuado en</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="1" i="0" u="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> el Inventario.</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-EC" sz="1100" b="1" i="0" u="none">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -4601,7 +4622,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>mide si se mantiene el nivel de existencias adecuado equivalente al 70 % para asegurar la disponibilidad continua de productos .</a:t>
+            <a:t>mide si se mantiene el nivel de existencias adecuado para asegurar la disponibilidad continua de productos.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4619,7 +4640,7 @@
             <a:t>Meta: </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-EC" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:rPr lang="es-EC" sz="1100" b="0" i="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -4628,13 +4649,11 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Mantener al menos 2 pacas de cada producto en inventario.</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-EC" b="0">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
+            <a:t>Mantener un nivel de existencias mayor al 70 %</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
           <a:r>
             <a:rPr lang="es-EC" sz="1100" b="1" i="0" baseline="0">
               <a:solidFill>
@@ -4647,12 +4666,10 @@
             </a:rPr>
             <a:t>Fórmula:</a:t>
           </a:r>
-          <a:endParaRPr lang="es-EC">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-EC" sz="1100" b="1" i="0" u="none">
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:endParaRPr lang="es-EC" sz="1100" b="1" i="0" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -4660,6 +4677,36 @@
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:endParaRPr lang="es-EC" sz="1100" b="1" i="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:endParaRPr lang="es-EC" sz="1100" b="1" i="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:endParaRPr lang="es-EC">
+            <a:effectLst/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -5084,7 +5131,43 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Errores en el cálculo de necesidades de reabastecimiento.</a:t>
+            <a:t>Un nivel de existencias bajo al</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>70</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> % indicara un desabastecimiento del inventario.</a:t>
           </a:r>
           <a:endParaRPr lang="es-EC" sz="1200" b="1" baseline="0"/>
         </a:p>
@@ -5674,15 +5757,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>73163</xdr:colOff>
+      <xdr:colOff>69619</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>115965</xdr:rowOff>
+      <xdr:rowOff>55714</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>537882</xdr:colOff>
+      <xdr:colOff>534338</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>100853</xdr:rowOff>
+      <xdr:rowOff>40602</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5712,8 +5795,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9161134" y="17272171"/>
-          <a:ext cx="2739513" cy="365888"/>
+          <a:off x="9419182" y="16681491"/>
+          <a:ext cx="2803882" cy="353483"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5765,7 +5848,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="MP14niveles!$C$9:$AY$85" spid="_x0000_s2094"/>
+                  <a14:cameraTool cellRange="MP14niveles!$C$9:$AY$85" spid="_x0000_s2098"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -6107,7 +6190,7 @@
   </sheetPr>
   <dimension ref="C12:AY86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M78" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AF77" zoomScale="215" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
       <selection activeCell="AF66" sqref="AF66"/>
     </sheetView>
   </sheetViews>
@@ -6232,14 +6315,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B370B9D439DDE546813D90F3B8B4DBAB" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="512b45069a73f00acf967ec99d7533f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xmlns:ns4="a8c64c2c-2712-4198-95b2-d256c44e1621" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5eb5ad93516d041cc0acfadbac38bba" ns3:_="" ns4:_="">
     <xsd:import namespace="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
@@ -6486,6 +6561,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6496,16 +6579,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E070C3-B3EF-4CFE-A975-5E4131163DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E52A94-29CD-49E2-93D5-AA07EA39528B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6524,6 +6597,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E070C3-B3EF-4CFE-A975-5E4131163DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8F17B7-1194-404B-B4BE-AE81FE298C94}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Mapa de proceso de 14 niveles ajustado a la correciones dadas
</commit_message>
<xml_diff>
--- a/01_Documentos/Grupo3_Mapa de procesos 14 niveles.xlsx
+++ b/01_Documentos/Grupo3_Mapa de procesos 14 niveles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivobook Oled\Desktop\Universidad\Septimo Semestre\Aseguramiento\Unidad 1\2563_G3_ACSW\01_Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATIAS\Desktop\ESPE\Septimo_Semestre\Quality Assurance\Repo\2563_G3_ACSW\01_Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B23B26-CEFB-4441-9081-CC991F2CEB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C079DA-B8CF-451A-9462-A66500ECCBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05AC8D40-0673-44FF-B842-F2CFFFBC4894}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{05AC8D40-0673-44FF-B842-F2CFFFBC4894}"/>
   </bookViews>
   <sheets>
     <sheet name="MP14niveles" sheetId="1" r:id="rId1"/>
@@ -3164,8 +3164,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9782453" y="8395750"/>
-          <a:ext cx="1360525" cy="1090818"/>
+          <a:off x="9546486" y="8724404"/>
+          <a:ext cx="1323440" cy="1140874"/>
           <a:chOff x="9484702" y="2765066"/>
           <a:chExt cx="1089646" cy="1074767"/>
         </a:xfrm>
@@ -4028,8 +4028,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7155866" y="5713212"/>
-          <a:ext cx="559827" cy="2386345"/>
+          <a:off x="7008225" y="5925066"/>
+          <a:ext cx="518023" cy="2494801"/>
           <a:chOff x="10126135" y="5820833"/>
           <a:chExt cx="533399" cy="2741084"/>
         </a:xfrm>
@@ -4205,8 +4205,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11078439" y="5735355"/>
-          <a:ext cx="559827" cy="2386345"/>
+          <a:off x="10842472" y="5947209"/>
+          <a:ext cx="518023" cy="2494801"/>
           <a:chOff x="10126135" y="5820833"/>
           <a:chExt cx="533399" cy="2741084"/>
         </a:xfrm>
@@ -5848,7 +5848,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="MP14niveles!$C$9:$AY$85" spid="_x0000_s2098"/>
+                  <a14:cameraTool cellRange="MP14niveles!$C$9:$AY$85" spid="_x0000_s2103"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -6190,50 +6190,50 @@
   </sheetPr>
   <dimension ref="C12:AY86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AF77" zoomScale="215" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="AF66" sqref="AF66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P73" zoomScale="89" zoomScaleNormal="89" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="X77" sqref="X77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="2.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
-    <col min="5" max="5" width="2.6640625" customWidth="1"/>
-    <col min="7" max="7" width="2.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="11" width="2.6640625" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" customWidth="1"/>
-    <col min="13" max="15" width="2.6640625" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
-    <col min="17" max="19" width="2.6640625" customWidth="1"/>
-    <col min="20" max="20" width="20.6640625" customWidth="1"/>
-    <col min="21" max="23" width="2.6640625" customWidth="1"/>
-    <col min="24" max="24" width="20.6640625" customWidth="1"/>
-    <col min="25" max="27" width="2.6640625" customWidth="1"/>
-    <col min="28" max="28" width="20.6640625" customWidth="1"/>
-    <col min="29" max="31" width="2.6640625" customWidth="1"/>
-    <col min="32" max="32" width="20.6640625" customWidth="1"/>
-    <col min="33" max="35" width="2.6640625" customWidth="1"/>
-    <col min="36" max="36" width="20.6640625" customWidth="1"/>
-    <col min="37" max="39" width="2.6640625" customWidth="1"/>
-    <col min="40" max="40" width="20.6640625" customWidth="1"/>
-    <col min="41" max="43" width="2.6640625" customWidth="1"/>
-    <col min="44" max="44" width="20.6640625" customWidth="1"/>
-    <col min="45" max="47" width="2.6640625" customWidth="1"/>
-    <col min="48" max="48" width="20.6640625" customWidth="1"/>
-    <col min="49" max="50" width="2.6640625" customWidth="1"/>
-    <col min="51" max="51" width="15.6640625" customWidth="1"/>
-    <col min="52" max="52" width="2.6640625" customWidth="1"/>
-    <col min="53" max="53" width="15.6640625" customWidth="1"/>
-    <col min="54" max="54" width="5.6640625" customWidth="1"/>
-    <col min="55" max="55" width="15.6640625" customWidth="1"/>
-    <col min="56" max="56" width="5.6640625" customWidth="1"/>
+    <col min="2" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="11" width="2.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="15" width="2.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="19" width="2.7109375" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
+    <col min="21" max="23" width="2.7109375" customWidth="1"/>
+    <col min="24" max="24" width="20.7109375" customWidth="1"/>
+    <col min="25" max="27" width="2.7109375" customWidth="1"/>
+    <col min="28" max="28" width="20.7109375" customWidth="1"/>
+    <col min="29" max="31" width="2.7109375" customWidth="1"/>
+    <col min="32" max="32" width="20.7109375" customWidth="1"/>
+    <col min="33" max="35" width="2.7109375" customWidth="1"/>
+    <col min="36" max="36" width="20.7109375" customWidth="1"/>
+    <col min="37" max="39" width="2.7109375" customWidth="1"/>
+    <col min="40" max="40" width="20.7109375" customWidth="1"/>
+    <col min="41" max="43" width="2.7109375" customWidth="1"/>
+    <col min="44" max="44" width="20.7109375" customWidth="1"/>
+    <col min="45" max="47" width="2.7109375" customWidth="1"/>
+    <col min="48" max="48" width="20.7109375" customWidth="1"/>
+    <col min="49" max="50" width="2.7109375" customWidth="1"/>
+    <col min="51" max="51" width="15.7109375" customWidth="1"/>
+    <col min="52" max="52" width="2.7109375" customWidth="1"/>
+    <col min="53" max="53" width="15.7109375" customWidth="1"/>
+    <col min="54" max="54" width="5.7109375" customWidth="1"/>
+    <col min="55" max="55" width="15.7109375" customWidth="1"/>
+    <col min="56" max="56" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="3:51" ht="8.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:51" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="3:51" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:51" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
@@ -6286,7 +6286,7 @@
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
     </row>
-    <row r="86" ht="8.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C13:AY13"/>
@@ -6306,7 +6306,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6315,6 +6315,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B370B9D439DDE546813D90F3B8B4DBAB" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="512b45069a73f00acf967ec99d7533f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xmlns:ns4="a8c64c2c-2712-4198-95b2-d256c44e1621" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5eb5ad93516d041cc0acfadbac38bba" ns3:_="" ns4:_="">
     <xsd:import namespace="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
@@ -6561,14 +6569,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6579,6 +6579,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E070C3-B3EF-4CFE-A975-5E4131163DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E52A94-29CD-49E2-93D5-AA07EA39528B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6597,16 +6607,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E070C3-B3EF-4CFE-A975-5E4131163DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b36d5ce4-fb93-4e20-ac5f-77871f6a1f70"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8F17B7-1194-404B-B4BE-AE81FE298C94}">
   <ds:schemaRefs>

</xml_diff>